<commit_message>
update xls to new ref api
</commit_message>
<xml_diff>
--- a/providers/excel-provider/src/test/resources/excell/TestData.xlsx
+++ b/providers/excel-provider/src/test/resources/excell/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clicm\sandbox\datajack\providers\excel-provider\src\test\resources\excell\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D579B6A4-157B-4689-BDDB-3F91AD60CA01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="18195" windowHeight="9525"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -68,9 +74,6 @@
     <t>linkToDiffSheet</t>
   </si>
   <si>
-    <t>link:DataBlocks.NewObject.VALUE</t>
-  </si>
-  <si>
     <t>NewObject</t>
   </si>
   <si>
@@ -119,36 +122,15 @@
     <t>cyclicRef</t>
   </si>
   <si>
-    <t>link:DataBlocks.AnotherObject.cyclicRef</t>
-  </si>
-  <si>
     <t>cyclic</t>
   </si>
   <si>
-    <t>link:Tests.Common.cyclic</t>
-  </si>
-  <si>
     <t>ref object data</t>
   </si>
   <si>
-    <t>link:DataBlocks.NewObject</t>
-  </si>
-  <si>
-    <t>link:Tests.Uncommon.reftest</t>
-  </si>
-  <si>
-    <t>link:Tests.Uncommon.reftestGen</t>
-  </si>
-  <si>
-    <t>link:DataBlocks.AnotherObject.anotherValue</t>
-  </si>
-  <si>
     <t>generatedInOtherCollection</t>
   </si>
   <si>
-    <t>link:Tests.Common.gendata</t>
-  </si>
-  <si>
     <t>MapTests</t>
   </si>
   <si>
@@ -180,12 +162,36 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>$ref:Tests:Uncommon.reftest</t>
+  </si>
+  <si>
+    <t>$ref:Tests:Uncommon.reftestGen</t>
+  </si>
+  <si>
+    <t>$ref:DataBlocks:AnotherObject.cyclicRef</t>
+  </si>
+  <si>
+    <t>$ref:DataBlocks:NewObject</t>
+  </si>
+  <si>
+    <t>$ref:DataBlocks:NewObject.VALUE</t>
+  </si>
+  <si>
+    <t>$ref:DataBlocks:AnotherObject.anotherValue</t>
+  </si>
+  <si>
+    <t>$ref:Tests:Common.cyclic</t>
+  </si>
+  <si>
+    <t>$ref:Tests:Common.gendata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -258,19 +264,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -280,7 +282,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -343,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,9 +378,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,6 +430,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -586,22 +622,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -615,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -623,7 +659,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -633,7 +669,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -643,65 +679,65 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -709,7 +745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -719,7 +755,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -729,93 +765,93 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7">
+        <v>42</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="1" t="s">
+      <c r="C20" s="8">
+        <v>42.1</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C21" s="9">
+        <v>42.21</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="9">
-        <v>42</v>
-      </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="10">
-        <v>42.1</v>
-      </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="11">
-        <v>42.21</v>
-      </c>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -824,80 +860,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>